<commit_message>
Updated first few entreis
</commit_message>
<xml_diff>
--- a/Qualitative_research/Research-Juvenile_Detention-New_col_added.xlsx
+++ b/Qualitative_research/Research-Juvenile_Detention-New_col_added.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\PhD\Internship\Loudoun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\VT DSPG\R files\2021_DSPG_Loudoun\Qualitative_research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A0209E-51D4-45E0-A2AB-7DA92F8693B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F828F2F3-6B03-4FC0-8BE5-EE7B97BFB36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="-12705" windowWidth="17190" windowHeight="10170" xr2:uid="{496A8450-741B-46B0-A040-55A896ED8080}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{496A8450-741B-46B0-A040-55A896ED8080}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="120">
   <si>
     <t>County</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Oxford House</t>
   </si>
   <si>
-    <t>Housing for those recovering from substance abuse</t>
-  </si>
-  <si>
     <t>Rapid Re-Housing Program</t>
   </si>
   <si>
@@ -99,16 +96,10 @@
     <t xml:space="preserve"> Provides job coaches who assist in finding and keeping regular jobs</t>
   </si>
   <si>
-    <t>Work In Loudoun Initiative</t>
-  </si>
-  <si>
     <t>Suite of job search services for Loudoun county jobs</t>
   </si>
   <si>
     <t>OAR</t>
-  </si>
-  <si>
-    <t>Works with those involved in the criminal justice system in Loudoun, Fairfax and Prince William County to provide post-release skill classes, community service substitutes for misdemeanor offers clothing, food, transportation, medication and violence prevention programs.</t>
   </si>
   <si>
     <t>Youth WIOA Program</t>
@@ -230,13 +221,201 @@
   </si>
   <si>
     <t>Office Location( Which Town, if no physical office address then "Online")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work In Loudoun Initiative </t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>18+</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>17+</t>
+  </si>
+  <si>
+    <t>https://www.loudoun.gov/1824/ADU-Purchase-Program</t>
+  </si>
+  <si>
+    <t>Shenandoah Building
+102 Heritage Way NE, Suite 103
+Leesburg, VA 20176</t>
+  </si>
+  <si>
+    <t>Loudoun County Family Services Department</t>
+  </si>
+  <si>
+    <t>39.114410, -77.540580</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Household must make between 30% and 70% of the median income in Loudoun, verification of identity and a mortgate loan pre-approval letter. </t>
+  </si>
+  <si>
+    <t>39.114410, -77.540581</t>
+  </si>
+  <si>
+    <t>Shenandoah Building
+102 Heritage Way NE, Suite 103
+Leesburg, VA 20177</t>
+  </si>
+  <si>
+    <t>Currently homeless or at risk of becoming homeless</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Those recovering from drug and alcohol addiction aiming to prevent relapse </t>
+  </si>
+  <si>
+    <t>Democratically run housing for those recovering from substance abuse who wish to be drug free and support others in their efforts</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>Oxford House World Services</t>
+  </si>
+  <si>
+    <t>Contact Us » Oxford Houses of Virginia (vaoxfordhouse.org)</t>
+  </si>
+  <si>
+    <t>Continuum of Care | Loudoun County, VA - Official Website</t>
+  </si>
+  <si>
+    <t>19520 Meadowview Court
+Leesburg, VA 20175</t>
+  </si>
+  <si>
+    <t>Volunteers of America Chesapeake</t>
+  </si>
+  <si>
+    <t>https://veteransnavigator.org/program/74824/loudoun-county-rapid-re-housing-program</t>
+  </si>
+  <si>
+    <t>39.076820, -77.549896</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resident of Loudoun County </t>
+  </si>
+  <si>
+    <t>Loudoun County Health and Human Services</t>
+  </si>
+  <si>
+    <t>Workforce Resource Center | Loudoun County, VA - Official Website</t>
+  </si>
+  <si>
+    <t>Unemployed or underemployed Loudoun County resident</t>
+  </si>
+  <si>
+    <t>Those searching for job in Loudoun County</t>
+  </si>
+  <si>
+    <t>1 Market St
+Leesburg, VA 20176</t>
+  </si>
+  <si>
+    <t>39.11528, -77.564430</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crossroads Jobs Inc. </t>
+  </si>
+  <si>
+    <t>https://crossroadsjobs.org/</t>
+  </si>
+  <si>
+    <t>906 Trailview Boulevard SE
+Suite A
+Leesburg, VA 20175</t>
+  </si>
+  <si>
+    <t>40.741895, -73.989308</t>
+  </si>
+  <si>
+    <t>https://www.loudoun.gov/1386/Employment-Services</t>
+  </si>
+  <si>
+    <t>Work In Loudoun, VA</t>
+  </si>
+  <si>
+    <t>Work in Loudoun - Loudoun County Economic Development, VA</t>
+  </si>
+  <si>
+    <t>26 Fairfax Street SE
+Suite 105
+Leesburg, VA 20175</t>
+  </si>
+  <si>
+    <t>39.1083999, -77.565337</t>
+  </si>
+  <si>
+    <t>Loudoun County (oarnova.org)</t>
+  </si>
+  <si>
+    <t>Those currently incarcerated or recently incarcerated</t>
+  </si>
+  <si>
+    <t>Works with those involved in the criminal justice system in Loudoun, Fairfax and Prince William County to provide employment assistance, post-release skill classes, community service substitutes for misdemeanor offers clothing, food, transportation, medication and violence prevention programs.</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>17-24</t>
+  </si>
+  <si>
+    <t>Those interested in gaining skills and education for success in the workforce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">102 Heritage Way, N.E. 
+1st Floor, Rear Entrance 
+Leesburg, VA 20176 </t>
+  </si>
+  <si>
+    <t>Virginia Career Works Northern Region</t>
+  </si>
+  <si>
+    <t>Contact - Virginia Career Works Northern Region (vcwnorthern.com)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loudoun County Public Schools </t>
+  </si>
+  <si>
+    <t>Instructional Programs / Adult Education (lcps.org)</t>
+  </si>
+  <si>
+    <t>39.115943, -77.581796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">715 Childrens Center Road
+Leesburg, VA 20175 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Those interested in continuing their education at a highschool level 18 and older </t>
+  </si>
+  <si>
+    <t>Low-Income adults and children interested in improving communication and literacy schools</t>
+  </si>
+  <si>
+    <t>199 Liberty Street SW, 3rd Floor
+Leesburg, VA 20175</t>
+  </si>
+  <si>
+    <t>Loudoun Literacy Council | Loudoun Literacy</t>
+  </si>
+  <si>
+    <t>39.1144062, -77.5677063</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +426,20 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -269,17 +462,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -594,29 +793,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B741EA-BD98-4FD7-9B1C-17627FF53E8A}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="24.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" customWidth="1"/>
-    <col min="4" max="4" width="54.6640625" customWidth="1"/>
-    <col min="5" max="5" width="23.109375" customWidth="1"/>
-    <col min="6" max="6" width="47.44140625" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="32" customWidth="1"/>
-    <col min="9" max="9" width="237.44140625" customWidth="1"/>
-    <col min="10" max="10" width="36.44140625" customWidth="1"/>
-    <col min="11" max="11" width="38.6640625" customWidth="1"/>
-    <col min="12" max="12" width="54.5546875" customWidth="1"/>
-    <col min="13" max="13" width="12.44140625"/>
+    <col min="1" max="2" width="24.90625" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" customWidth="1"/>
+    <col min="4" max="4" width="54.6328125" customWidth="1"/>
+    <col min="5" max="5" width="23.08984375" customWidth="1"/>
+    <col min="6" max="6" width="47.453125" customWidth="1"/>
+    <col min="7" max="7" width="18.36328125" customWidth="1"/>
+    <col min="8" max="8" width="135.54296875" customWidth="1"/>
+    <col min="9" max="9" width="70.90625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="130.6328125" customWidth="1"/>
+    <col min="11" max="11" width="107.90625" customWidth="1"/>
+    <col min="12" max="12" width="99.81640625" customWidth="1"/>
+    <col min="13" max="13" width="62.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -631,31 +830,31 @@
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -669,13 +868,34 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -689,13 +909,34 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L3" t="s">
+        <v>70</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -709,13 +950,34 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="F4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K4" t="s">
+        <v>78</v>
+      </c>
+      <c r="L4" t="s">
+        <v>79</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -726,16 +988,37 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
-        <v>54</v>
-      </c>
-      <c r="I5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J5" t="s">
+        <v>85</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L5" t="s">
+        <v>83</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -743,19 +1026,40 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="s">
-        <v>54</v>
-      </c>
-      <c r="I6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J6" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L6" t="s">
+        <v>87</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -763,19 +1067,40 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E7" t="s">
-        <v>54</v>
-      </c>
-      <c r="I7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L7" t="s">
+        <v>93</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -783,19 +1108,40 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" t="s">
+        <v>90</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E8" t="s">
-        <v>54</v>
-      </c>
-      <c r="I8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J8" t="s">
+        <v>96</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="L8" t="s">
+        <v>87</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -803,59 +1149,122 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
-      </c>
-      <c r="I9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="F9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" t="s">
+        <v>105</v>
+      </c>
+      <c r="H9" t="s">
+        <v>90</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" t="s">
+        <v>78</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L9" t="s">
+        <v>98</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
-      </c>
-      <c r="I10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="F10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" t="s">
+        <v>103</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J10" t="s">
+        <v>101</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="L10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
-      </c>
-      <c r="I11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="F11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" t="s">
+        <v>106</v>
+      </c>
+      <c r="H11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" t="s">
+        <v>71</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L11" t="s">
+        <v>109</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -863,19 +1272,40 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>51</v>
+      </c>
+      <c r="F12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" t="s">
+        <v>115</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="J12" t="s">
+        <v>113</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L12" t="s">
+        <v>111</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -883,254 +1313,312 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" t="s">
-        <v>30</v>
-      </c>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="F13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" t="s">
-        <v>33</v>
+      <c r="I14" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
         <v>31</v>
       </c>
-      <c r="C15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" t="s">
-        <v>34</v>
-      </c>
       <c r="E15" t="s">
-        <v>54</v>
-      </c>
-      <c r="I15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
-      </c>
-      <c r="I16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="F16" t="s">
+        <v>64</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
-      </c>
-      <c r="I17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="F17" t="s">
+        <v>64</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" t="s">
+        <v>64</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D18" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" t="s">
-        <v>54</v>
-      </c>
-      <c r="I18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
-      </c>
-      <c r="I19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="F19" t="s">
+        <v>64</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
-      </c>
-      <c r="I20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="F20" t="s">
+        <v>64</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
-      </c>
-      <c r="I21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="F21" t="s">
+        <v>64</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D22" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E22" t="s">
-        <v>54</v>
-      </c>
-      <c r="I22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="F22" t="s">
+        <v>64</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E23" t="s">
-        <v>54</v>
-      </c>
-      <c r="I23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="F23" t="s">
+        <v>64</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D24" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E24" t="s">
-        <v>54</v>
-      </c>
-      <c r="I24" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="F24" t="s">
+        <v>64</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{32466310-BBD0-4391-A010-F8E2F159CEB0}"/>
+    <hyperlink ref="M4" r:id="rId2" display="https://www.vaoxfordhouse.org/contact-us/" xr:uid="{55EFA22F-D97E-4D61-973D-3CC5441130CA}"/>
+    <hyperlink ref="M3" r:id="rId3" display="https://www.loudoun.gov/CoC" xr:uid="{E276024C-43D3-4D20-A390-1EC4D70FFB6A}"/>
+    <hyperlink ref="M5" r:id="rId4" xr:uid="{A9CA4265-2C8F-416A-B9E2-99592ED7241A}"/>
+    <hyperlink ref="M6" r:id="rId5" display="https://www.loudoun.gov/1592/Workforce-Resource-Center" xr:uid="{3023DCB6-B6DF-4715-B21D-D5E8A888AC3A}"/>
+    <hyperlink ref="M7" r:id="rId6" xr:uid="{8516C3D7-00E9-43FB-83B8-B35F4788F110}"/>
+    <hyperlink ref="M8" r:id="rId7" xr:uid="{3FEC7435-8C7C-480B-AC49-9463843EABA1}"/>
+    <hyperlink ref="M9" r:id="rId8" display="https://biz.loudoun.gov/work-in-loudoun/" xr:uid="{3CD91D4D-690A-45E1-B334-22F91CABCBD9}"/>
+    <hyperlink ref="M10" r:id="rId9" display="https://www.oarnova.org/services/loudoun-county" xr:uid="{0CFB1529-CA93-4247-ABEE-73F22F189349}"/>
+    <hyperlink ref="M11" r:id="rId10" display="https://vcwnorthern.com/contact/" xr:uid="{72646037-B63C-4C8B-8891-AF7F215DBFA1}"/>
+    <hyperlink ref="M12" r:id="rId11" display="https://www.lcps.org/adulted" xr:uid="{41EBE335-8913-4C80-8F8F-7D6B310D4DC1}"/>
+    <hyperlink ref="M13" r:id="rId12" display="https://loudounliteracy.org/" xr:uid="{BE17D43A-8109-417C-88B6-F74BD000FCCC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Spreadsheet and Rmd file
</commit_message>
<xml_diff>
--- a/Qualitative_research/Research-Juvenile_Detention-New_col_added.xlsx
+++ b/Qualitative_research/Research-Juvenile_Detention-New_col_added.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\VT DSPG\R files\2021_DSPG_Loudoun\Qualitative_research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F828F2F3-6B03-4FC0-8BE5-EE7B97BFB36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FAD2F3-64A7-4813-B1D6-B00DFED9F672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{496A8450-741B-46B0-A040-55A896ED8080}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="153">
   <si>
     <t>County</t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t>Partner4Work</t>
-  </si>
-  <si>
-    <t>Offers a variety of career development programs and services for disadvantaged young adults with and without GEDs</t>
   </si>
   <si>
     <t>Career Pipeline Program</t>
@@ -255,9 +252,6 @@
     <t>39.114410, -77.540580</t>
   </si>
   <si>
-    <t xml:space="preserve">Household must make between 30% and 70% of the median income in Loudoun, verification of identity and a mortgate loan pre-approval letter. </t>
-  </si>
-  <si>
     <t>39.114410, -77.540581</t>
   </si>
   <si>
@@ -266,9 +260,6 @@
 Leesburg, VA 20177</t>
   </si>
   <si>
-    <t>Currently homeless or at risk of becoming homeless</t>
-  </si>
-  <si>
     <t xml:space="preserve">Those recovering from drug and alcohol addiction aiming to prevent relapse </t>
   </si>
   <si>
@@ -409,13 +400,125 @@
   </si>
   <si>
     <t>39.1144062, -77.5677063</t>
+  </si>
+  <si>
+    <t>18-24</t>
+  </si>
+  <si>
+    <t>14-21</t>
+  </si>
+  <si>
+    <t>Pennsylvania youth aged 18-24 experiencing housing inequality in Allegheny, Armstrong and Westmoreland(16-24)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valley Youth House </t>
+  </si>
+  <si>
+    <t>Bridge2Home Host Homes - Valley Youth House</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allegheny residents at risk of becoming homeless </t>
+  </si>
+  <si>
+    <t>One Smithfield Street, Pittsburgh 15222</t>
+  </si>
+  <si>
+    <t>40.43978, -79.998870</t>
+  </si>
+  <si>
+    <t>18-24 year olds who are or have been involved in the justice system in Allegheny County</t>
+  </si>
+  <si>
+    <t>https://www.partner4work.org/programs/career-pipeline-project/</t>
+  </si>
+  <si>
+    <t>Reentry Programs - Partner4Work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18+ </t>
+  </si>
+  <si>
+    <t>Those with multiple barriers to gaining employment</t>
+  </si>
+  <si>
+    <t>Low-Income young adults residing in Allegheny County</t>
+  </si>
+  <si>
+    <t>Learn &amp; Earn / Learn &amp; Earn (general program) - Partner4Work</t>
+  </si>
+  <si>
+    <t>Learn &amp; Earn / Learn &amp; Earn Corporate Internship Program - Partner4Work</t>
+  </si>
+  <si>
+    <t>Those in need of job assistance in Allegheny County</t>
+  </si>
+  <si>
+    <t>Mon Valley Initiative
+305 E. Eighth Ave.
+Homestead, PA 15120</t>
+  </si>
+  <si>
+    <t>40.40796,-79.909258</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mon Valley Initiative </t>
+  </si>
+  <si>
+    <t>Finding a Job - (monvalleyinitiative.com)</t>
+  </si>
+  <si>
+    <t>Supports for Success | HSCC (hscc-mvpc.org)</t>
+  </si>
+  <si>
+    <t>Human Services Center Corporation</t>
+  </si>
+  <si>
+    <t>519 Penn Avenue, Turtle Creek, PA 15145</t>
+  </si>
+  <si>
+    <t>40.4052591,-79.8291844</t>
+  </si>
+  <si>
+    <t>Must make 200% of the federal poverty level or less, have a goal of employment/education, live within Mon Valley (in Allegheny)</t>
+  </si>
+  <si>
+    <t>Employment Services — North Hills Community Outreach (nhco.org)</t>
+  </si>
+  <si>
+    <t>1975 Ferguson Road
+Allison Park, PA 15101
+412-487-6316</t>
+  </si>
+  <si>
+    <t>40.55951,-79.95867</t>
+  </si>
+  <si>
+    <t>North Hills Community Outreach</t>
+  </si>
+  <si>
+    <t>Allegheny County Resident</t>
+  </si>
+  <si>
+    <t>Allegheny Link to Aging and Disability Resources (alleghenycounty.us)</t>
+  </si>
+  <si>
+    <t>Allegheny County Department of Human Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Household must make between 30% and 70% of the median income in Loudoun, verification of identity available and a mortgate loan pre-approval letter must be obtained. </t>
+  </si>
+  <si>
+    <t>Those currently homeless or at risk of becoming homeless</t>
+  </si>
+  <si>
+    <t>Those searching for a job in Loudoun County</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -444,6 +547,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -466,7 +575,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -476,6 +585,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -791,10 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B741EA-BD98-4FD7-9B1C-17627FF53E8A}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -805,17 +915,17 @@
     <col min="5" max="5" width="23.08984375" customWidth="1"/>
     <col min="6" max="6" width="47.453125" customWidth="1"/>
     <col min="7" max="7" width="18.36328125" customWidth="1"/>
-    <col min="8" max="8" width="135.54296875" customWidth="1"/>
+    <col min="8" max="8" width="144.81640625" customWidth="1"/>
     <col min="9" max="9" width="70.90625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="130.6328125" customWidth="1"/>
-    <col min="11" max="11" width="107.90625" customWidth="1"/>
+    <col min="10" max="10" width="115.7265625" customWidth="1"/>
+    <col min="11" max="11" width="116.1796875" customWidth="1"/>
     <col min="12" max="12" width="99.81640625" customWidth="1"/>
     <col min="13" max="13" width="62.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -830,28 +940,28 @@
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="L1" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
@@ -868,31 +978,31 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H2" t="s">
-        <v>72</v>
+        <v>150</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L2" t="s">
         <v>69</v>
       </c>
-      <c r="L2" t="s">
-        <v>70</v>
-      </c>
       <c r="M2" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
@@ -909,31 +1019,31 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H3" t="s">
-        <v>75</v>
+        <v>151</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
@@ -950,31 +1060,31 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K4" t="s">
+        <v>75</v>
+      </c>
+      <c r="L4" t="s">
         <v>76</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="M4" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="J4" t="s">
-        <v>78</v>
-      </c>
-      <c r="K4" t="s">
-        <v>78</v>
-      </c>
-      <c r="L4" t="s">
-        <v>79</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
@@ -991,31 +1101,31 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="L5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="29" x14ac:dyDescent="0.35">
@@ -1026,37 +1136,37 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="29" x14ac:dyDescent="0.35">
@@ -1067,37 +1177,37 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L7" t="s">
+        <v>90</v>
+      </c>
+      <c r="M7" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="L7" t="s">
-        <v>93</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
@@ -1108,37 +1218,37 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
         <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H8" t="s">
-        <v>90</v>
+        <v>152</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="L8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
@@ -1149,37 +1259,37 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" t="s">
         <v>62</v>
       </c>
-      <c r="E9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" t="s">
-        <v>63</v>
-      </c>
       <c r="G9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H9" t="s">
-        <v>90</v>
+        <v>152</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="L9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="58" x14ac:dyDescent="0.35">
@@ -1187,40 +1297,40 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
         <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" t="s">
         <v>64</v>
       </c>
-      <c r="G10" t="s">
-        <v>65</v>
-      </c>
       <c r="H10" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L10" t="s">
         <v>21</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
@@ -1228,40 +1338,40 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="J11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="L11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="58" x14ac:dyDescent="0.35">
@@ -1272,37 +1382,37 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
         <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>25</v>
       </c>
       <c r="J12" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="L12" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
@@ -1313,37 +1423,37 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
         <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>26</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
@@ -1354,26 +1464,38 @@
         <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
         <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="I14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
+      <c r="J14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
@@ -1383,223 +1505,359 @@
         <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
         <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="F15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" t="s">
+        <v>122</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="J15" t="s">
+        <v>124</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="L15" t="s">
+        <v>149</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
         <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" t="s">
+        <v>117</v>
+      </c>
+      <c r="H16" t="s">
+        <v>125</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J16" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L16" t="s">
         <v>33</v>
       </c>
-      <c r="E16" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" t="s">
-        <v>64</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="M16" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
         <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F17" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="G17" t="s">
+        <v>117</v>
+      </c>
+      <c r="H17" t="s">
+        <v>125</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+      <c r="J17" t="s">
+        <v>75</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L17" t="s">
+        <v>33</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
         <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
         <v>37</v>
       </c>
       <c r="E18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F18" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="G18" t="s">
+        <v>128</v>
+      </c>
+      <c r="H18" t="s">
+        <v>129</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+      <c r="J18" t="s">
+        <v>75</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
         <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F19" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="G19" t="s">
+        <v>118</v>
+      </c>
+      <c r="H19" t="s">
+        <v>130</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="J19" t="s">
+        <v>75</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L19" t="s">
+        <v>33</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
         <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F20" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="G20" t="s">
+        <v>117</v>
+      </c>
+      <c r="H20" t="s">
+        <v>130</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+      <c r="L20" t="s">
+        <v>33</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F21" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="G21" t="s">
+        <v>128</v>
+      </c>
+      <c r="H21" t="s">
+        <v>133</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+      <c r="J21" t="s">
+        <v>135</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="L21" t="s">
+        <v>136</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
         <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" t="s">
         <v>64</v>
       </c>
+      <c r="H22" t="s">
+        <v>142</v>
+      </c>
       <c r="I22" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+      <c r="J22" t="s">
+        <v>141</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="L22" t="s">
+        <v>139</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
         <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D23" t="s">
         <v>46</v>
       </c>
       <c r="E23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F23" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="G23" t="s">
+        <v>65</v>
+      </c>
+      <c r="H23" t="s">
+        <v>147</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" t="s">
-        <v>51</v>
-      </c>
-      <c r="F24" t="s">
-        <v>64</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>49</v>
+      <c r="J23" t="s">
+        <v>145</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="L23" t="s">
+        <v>146</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1617,8 +1875,18 @@
     <hyperlink ref="M11" r:id="rId10" display="https://vcwnorthern.com/contact/" xr:uid="{72646037-B63C-4C8B-8891-AF7F215DBFA1}"/>
     <hyperlink ref="M12" r:id="rId11" display="https://www.lcps.org/adulted" xr:uid="{41EBE335-8913-4C80-8F8F-7D6B310D4DC1}"/>
     <hyperlink ref="M13" r:id="rId12" display="https://loudounliteracy.org/" xr:uid="{BE17D43A-8109-417C-88B6-F74BD000FCCC}"/>
+    <hyperlink ref="M14" r:id="rId13" display="https://www.valleyyouthhouse.org/programs/transitional-housing/bridge2home-host-homes/" xr:uid="{FF2C999A-7A0E-49D4-8B95-BA6FE062A76D}"/>
+    <hyperlink ref="M16" r:id="rId14" xr:uid="{99CF2C95-5FF3-44E6-A6EB-1BBF370DF25B}"/>
+    <hyperlink ref="M17" r:id="rId15" display="https://www.partner4work.org/programs/strive/" xr:uid="{5644EC3E-041B-4CD0-BCB5-540C17241997}"/>
+    <hyperlink ref="M19" r:id="rId16" display="https://www.partner4work.org/learn-and-earn/" xr:uid="{7F2CFB56-C4D1-41B8-8DC5-5E97433251C2}"/>
+    <hyperlink ref="M18" r:id="rId17" display="https://www.partner4work.org/programs/transitional-jobs/" xr:uid="{69748E6B-1AD4-45BF-9F21-92B93F97803C}"/>
+    <hyperlink ref="M20" r:id="rId18" display="https://www.partner4work.org/corporate-internship-program" xr:uid="{73418219-6B1C-4901-8E75-2F2FEA2A9FCF}"/>
+    <hyperlink ref="M21" r:id="rId19" display="https://monvalleyinitiative.com/get-help-with/finding-a-job/" xr:uid="{6F25D67C-206A-46FA-98B4-CF7DE2B7BD36}"/>
+    <hyperlink ref="M22" r:id="rId20" display="https://hscc-mvpc.org/community-programs/supports-for-success/" xr:uid="{BD8C2F79-668D-4464-8C3C-15D248E2B06F}"/>
+    <hyperlink ref="M23" r:id="rId21" display="https://www.nhco.org/employment-services" xr:uid="{E29FB4DF-669A-4622-A7DD-F11E5C925BCA}"/>
+    <hyperlink ref="M15" r:id="rId22" display="https://www.alleghenycounty.us/Human-Services/About/Contact/Allegheny-Link.aspx" xr:uid="{3B69D816-F50B-4FB6-B94F-647FF0F58081}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated excel file, added Allegheny County transportation and health care info
</commit_message>
<xml_diff>
--- a/Qualitative_research/Research-Juvenile_Detention-New_col_added.xlsx
+++ b/Qualitative_research/Research-Juvenile_Detention-New_col_added.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\VT DSPG\R files\2021_DSPG_Loudoun\Qualitative_research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FAD2F3-64A7-4813-B1D6-B00DFED9F672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C141A4B1-DC64-458A-86FC-1DD5304F809A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{496A8450-741B-46B0-A040-55A896ED8080}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="173">
   <si>
     <t>County</t>
   </si>
@@ -512,6 +512,66 @@
   </si>
   <si>
     <t>Those searching for a job in Loudoun County</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Education </t>
+  </si>
+  <si>
+    <t>DHS Education Liaison</t>
+  </si>
+  <si>
+    <t>CCAC Workforce Development Program</t>
+  </si>
+  <si>
+    <t>CCAC Apprenticeship Programs</t>
+  </si>
+  <si>
+    <t>CCAC Commonwealth Diploma Program</t>
+  </si>
+  <si>
+    <t>CCAC KEYS Program</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>Port Authority Allegheny County</t>
+  </si>
+  <si>
+    <t>Medical Assistance Transportation Program</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Health Choices</t>
+  </si>
+  <si>
+    <t>Mental Health Rx Pharmacy Benefit Program</t>
+  </si>
+  <si>
+    <t>Virginia Medicaid</t>
+  </si>
+  <si>
+    <t>Loudoun Free Clinic</t>
+  </si>
+  <si>
+    <t>Loudoun County Local Bus Service</t>
+  </si>
+  <si>
+    <t>Medicaid Transportation</t>
+  </si>
+  <si>
+    <t>Care Mobile Tranportation</t>
+  </si>
+  <si>
+    <t>Loudoun County Commuter and Metro Connect Bus Services</t>
+  </si>
+  <si>
+    <t>19-64</t>
   </si>
 </sst>
 </file>
@@ -901,10 +961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B741EA-BD98-4FD7-9B1C-17627FF53E8A}">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1382,7 +1442,7 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>153</v>
       </c>
       <c r="D12" t="s">
         <v>24</v>
@@ -1423,7 +1483,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>153</v>
       </c>
       <c r="D13" t="s">
         <v>26</v>
@@ -1457,58 +1517,34 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>13</v>
-      </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>163</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>166</v>
       </c>
       <c r="E14" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>121</v>
+      <c r="F14" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>14</v>
-      </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>163</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>167</v>
       </c>
       <c r="E15" t="s">
         <v>50</v>
@@ -1516,348 +1552,628 @@
       <c r="F15" t="s">
         <v>62</v>
       </c>
-      <c r="G15" t="s">
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>160</v>
+      </c>
+      <c r="D16" t="s">
+        <v>168</v>
+      </c>
+      <c r="E16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>160</v>
+      </c>
+      <c r="D17" t="s">
+        <v>169</v>
+      </c>
+      <c r="E17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>160</v>
+      </c>
+      <c r="D18" t="s">
+        <v>170</v>
+      </c>
+      <c r="E18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>160</v>
+      </c>
+      <c r="D19" t="s">
+        <v>171</v>
+      </c>
+      <c r="E19" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="E20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="E21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="E22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="E23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="E24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" t="s">
+        <v>62</v>
+      </c>
+      <c r="G26" t="s">
         <v>65</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H26" t="s">
         <v>122</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J26" t="s">
         <v>124</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L26" t="s">
         <v>149</v>
       </c>
-      <c r="M15" s="4" t="s">
+      <c r="M26" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16">
+    <row r="27" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A27">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B27" t="s">
         <v>28</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C27" t="s">
         <v>49</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D27" t="s">
         <v>34</v>
       </c>
-      <c r="E16" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="E27" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" t="s">
         <v>63</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G27" t="s">
         <v>117</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H27" t="s">
         <v>125</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J27" t="s">
         <v>75</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L27" t="s">
         <v>33</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="M27" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17">
+    <row r="28" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A28">
         <v>17</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B28" t="s">
         <v>28</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C28" t="s">
         <v>49</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D28" t="s">
         <v>36</v>
       </c>
-      <c r="E17" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="E28" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" t="s">
         <v>63</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G28" t="s">
         <v>117</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H28" t="s">
         <v>125</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J28" t="s">
         <v>75</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L28" t="s">
         <v>33</v>
       </c>
-      <c r="M17" s="4" t="s">
+      <c r="M28" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18">
+    <row r="29" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29">
         <v>18</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B29" t="s">
         <v>28</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C29" t="s">
         <v>49</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D29" t="s">
         <v>37</v>
       </c>
-      <c r="E18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="E29" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" t="s">
         <v>63</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G29" t="s">
         <v>128</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H29" t="s">
         <v>129</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J29" t="s">
         <v>75</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L29" t="s">
         <v>33</v>
       </c>
-      <c r="M18" s="4" t="s">
+      <c r="M29" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19">
+    <row r="30" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30">
         <v>19</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B30" t="s">
         <v>28</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C30" t="s">
         <v>49</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D30" t="s">
         <v>39</v>
       </c>
-      <c r="E19" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="E30" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" t="s">
         <v>63</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G30" t="s">
         <v>118</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H30" t="s">
         <v>130</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I30" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J30" t="s">
         <v>75</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L30" t="s">
         <v>33</v>
       </c>
-      <c r="M19" s="4" t="s">
+      <c r="M30" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A31">
         <v>20</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B31" t="s">
         <v>28</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C31" t="s">
         <v>49</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D31" t="s">
         <v>41</v>
       </c>
-      <c r="E20" t="s">
-        <v>50</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="E31" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" t="s">
         <v>63</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G31" t="s">
         <v>117</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H31" t="s">
         <v>130</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L31" t="s">
         <v>33</v>
       </c>
-      <c r="M20" s="4" t="s">
+      <c r="M31" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21">
+    <row r="32" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A32">
         <v>21</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B32" t="s">
         <v>28</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C32" t="s">
         <v>49</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D32" t="s">
         <v>43</v>
       </c>
-      <c r="E21" t="s">
-        <v>50</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="E32" t="s">
+        <v>50</v>
+      </c>
+      <c r="F32" t="s">
         <v>62</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G32" t="s">
         <v>128</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H32" t="s">
         <v>133</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J32" t="s">
         <v>135</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="K32" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="L21" t="s">
+      <c r="L32" t="s">
         <v>136</v>
       </c>
-      <c r="M21" s="4" t="s">
+      <c r="M32" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22">
+    <row r="33" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33">
         <v>22</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B33" t="s">
         <v>28</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C33" t="s">
         <v>49</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D33" t="s">
         <v>45</v>
       </c>
-      <c r="E22" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="E33" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" t="s">
         <v>62</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G33" t="s">
         <v>64</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H33" t="s">
         <v>142</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J33" t="s">
         <v>141</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="K33" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L33" t="s">
         <v>139</v>
       </c>
-      <c r="M22" s="4" t="s">
+      <c r="M33" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A23">
+    <row r="34" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A34">
         <v>23</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B34" t="s">
         <v>28</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C34" t="s">
         <v>49</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D34" t="s">
         <v>46</v>
       </c>
-      <c r="E23" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="E34" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34" t="s">
         <v>62</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G34" t="s">
         <v>65</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H34" t="s">
         <v>147</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J34" t="s">
         <v>145</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="K34" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="L23" t="s">
+      <c r="L34" t="s">
         <v>146</v>
       </c>
-      <c r="M23" s="4" t="s">
+      <c r="M34" s="4" t="s">
         <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>24</v>
+      </c>
+      <c r="B35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" t="s">
+        <v>154</v>
+      </c>
+      <c r="D35" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>25</v>
+      </c>
+      <c r="B36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" t="s">
+        <v>154</v>
+      </c>
+      <c r="D36" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>26</v>
+      </c>
+      <c r="B37" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" t="s">
+        <v>154</v>
+      </c>
+      <c r="D37" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>27</v>
+      </c>
+      <c r="B38" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" t="s">
+        <v>154</v>
+      </c>
+      <c r="D38" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>28</v>
+      </c>
+      <c r="B39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" t="s">
+        <v>154</v>
+      </c>
+      <c r="D39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>29</v>
+      </c>
+      <c r="B40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" t="s">
+        <v>160</v>
+      </c>
+      <c r="D40" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>30</v>
+      </c>
+      <c r="B41" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" t="s">
+        <v>160</v>
+      </c>
+      <c r="D41" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>31</v>
+      </c>
+      <c r="B42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" t="s">
+        <v>163</v>
+      </c>
+      <c r="D42" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>32</v>
+      </c>
+      <c r="B43" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" t="s">
+        <v>163</v>
+      </c>
+      <c r="D43" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -1875,16 +2191,16 @@
     <hyperlink ref="M11" r:id="rId10" display="https://vcwnorthern.com/contact/" xr:uid="{72646037-B63C-4C8B-8891-AF7F215DBFA1}"/>
     <hyperlink ref="M12" r:id="rId11" display="https://www.lcps.org/adulted" xr:uid="{41EBE335-8913-4C80-8F8F-7D6B310D4DC1}"/>
     <hyperlink ref="M13" r:id="rId12" display="https://loudounliteracy.org/" xr:uid="{BE17D43A-8109-417C-88B6-F74BD000FCCC}"/>
-    <hyperlink ref="M14" r:id="rId13" display="https://www.valleyyouthhouse.org/programs/transitional-housing/bridge2home-host-homes/" xr:uid="{FF2C999A-7A0E-49D4-8B95-BA6FE062A76D}"/>
-    <hyperlink ref="M16" r:id="rId14" xr:uid="{99CF2C95-5FF3-44E6-A6EB-1BBF370DF25B}"/>
-    <hyperlink ref="M17" r:id="rId15" display="https://www.partner4work.org/programs/strive/" xr:uid="{5644EC3E-041B-4CD0-BCB5-540C17241997}"/>
-    <hyperlink ref="M19" r:id="rId16" display="https://www.partner4work.org/learn-and-earn/" xr:uid="{7F2CFB56-C4D1-41B8-8DC5-5E97433251C2}"/>
-    <hyperlink ref="M18" r:id="rId17" display="https://www.partner4work.org/programs/transitional-jobs/" xr:uid="{69748E6B-1AD4-45BF-9F21-92B93F97803C}"/>
-    <hyperlink ref="M20" r:id="rId18" display="https://www.partner4work.org/corporate-internship-program" xr:uid="{73418219-6B1C-4901-8E75-2F2FEA2A9FCF}"/>
-    <hyperlink ref="M21" r:id="rId19" display="https://monvalleyinitiative.com/get-help-with/finding-a-job/" xr:uid="{6F25D67C-206A-46FA-98B4-CF7DE2B7BD36}"/>
-    <hyperlink ref="M22" r:id="rId20" display="https://hscc-mvpc.org/community-programs/supports-for-success/" xr:uid="{BD8C2F79-668D-4464-8C3C-15D248E2B06F}"/>
-    <hyperlink ref="M23" r:id="rId21" display="https://www.nhco.org/employment-services" xr:uid="{E29FB4DF-669A-4622-A7DD-F11E5C925BCA}"/>
-    <hyperlink ref="M15" r:id="rId22" display="https://www.alleghenycounty.us/Human-Services/About/Contact/Allegheny-Link.aspx" xr:uid="{3B69D816-F50B-4FB6-B94F-647FF0F58081}"/>
+    <hyperlink ref="M25" r:id="rId13" display="https://www.valleyyouthhouse.org/programs/transitional-housing/bridge2home-host-homes/" xr:uid="{FF2C999A-7A0E-49D4-8B95-BA6FE062A76D}"/>
+    <hyperlink ref="M27" r:id="rId14" xr:uid="{99CF2C95-5FF3-44E6-A6EB-1BBF370DF25B}"/>
+    <hyperlink ref="M28" r:id="rId15" display="https://www.partner4work.org/programs/strive/" xr:uid="{5644EC3E-041B-4CD0-BCB5-540C17241997}"/>
+    <hyperlink ref="M30" r:id="rId16" display="https://www.partner4work.org/learn-and-earn/" xr:uid="{7F2CFB56-C4D1-41B8-8DC5-5E97433251C2}"/>
+    <hyperlink ref="M29" r:id="rId17" display="https://www.partner4work.org/programs/transitional-jobs/" xr:uid="{69748E6B-1AD4-45BF-9F21-92B93F97803C}"/>
+    <hyperlink ref="M31" r:id="rId18" display="https://www.partner4work.org/corporate-internship-program" xr:uid="{73418219-6B1C-4901-8E75-2F2FEA2A9FCF}"/>
+    <hyperlink ref="M32" r:id="rId19" display="https://monvalleyinitiative.com/get-help-with/finding-a-job/" xr:uid="{6F25D67C-206A-46FA-98B4-CF7DE2B7BD36}"/>
+    <hyperlink ref="M33" r:id="rId20" display="https://hscc-mvpc.org/community-programs/supports-for-success/" xr:uid="{BD8C2F79-668D-4464-8C3C-15D248E2B06F}"/>
+    <hyperlink ref="M34" r:id="rId21" display="https://www.nhco.org/employment-services" xr:uid="{E29FB4DF-669A-4622-A7DD-F11E5C925BCA}"/>
+    <hyperlink ref="M26" r:id="rId22" display="https://www.alleghenycounty.us/Human-Services/About/Contact/Allegheny-Link.aspx" xr:uid="{3B69D816-F50B-4FB6-B94F-647FF0F58081}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId23"/>

</xml_diff>

<commit_message>
Updated Pillars for consistent naming convention, updated map to be more consistent
</commit_message>
<xml_diff>
--- a/Qualitative_research/Research-Juvenile_Detention-New_col_added.xlsx
+++ b/Qualitative_research/Research-Juvenile_Detention-New_col_added.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\VT DSPG\R files\2021_DSPG_Loudoun\Qualitative_research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CBFF8ED-6AF5-489A-8119-45E04559737E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A99D02C-4655-43B6-AC10-CD6C6F3C4F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{496A8450-741B-46B0-A040-55A896ED8080}"/>
   </bookViews>
@@ -76,9 +76,6 @@
     <t>Loudoun</t>
   </si>
   <si>
-    <t>Housing Services</t>
-  </si>
-  <si>
     <t>Loudoun County Affordable Dwelling Unit Program</t>
   </si>
   <si>
@@ -155,9 +152,6 @@
     <t>Alleghany Link</t>
   </si>
   <si>
-    <t>Offers a variety of housing services to those at risk for homelessness</t>
-  </si>
-  <si>
     <t>Partner4Work</t>
   </si>
   <si>
@@ -580,6 +574,12 @@
   </si>
   <si>
     <t>http://www.caremobiletransportation.com/our-history</t>
+  </si>
+  <si>
+    <t>Housing</t>
+  </si>
+  <si>
+    <t>Offers a variety of Housing to those at risk for homelessness</t>
   </si>
 </sst>
 </file>
@@ -981,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B741EA-BD98-4FD7-9B1C-17627FF53E8A}">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M15" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1003,7 +1003,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1018,31 +1018,31 @@
         <v>1</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
@@ -1054,25 +1054,25 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="J2" s="3">
         <v>39.114409999999999</v>
@@ -1081,13 +1081,13 @@
         <v>-77.540580000000006</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="31" x14ac:dyDescent="0.35">
@@ -1098,25 +1098,25 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="J3" s="3">
         <v>39.114409999999999</v>
@@ -1125,13 +1125,13 @@
         <v>-77.540581000000003</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="31" x14ac:dyDescent="0.35">
@@ -1142,40 +1142,40 @@
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="K4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="N4" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="31" x14ac:dyDescent="0.35">
@@ -1186,25 +1186,25 @@
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="J5" s="3">
         <v>39.076819999999998</v>
@@ -1213,13 +1213,13 @@
         <v>-77.549896000000004</v>
       </c>
       <c r="L5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="N5" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="31" x14ac:dyDescent="0.35">
@@ -1230,25 +1230,25 @@
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="J6" s="3">
         <v>39.114409999999999</v>
@@ -1257,13 +1257,13 @@
         <v>-77.540581000000003</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="31" x14ac:dyDescent="0.35">
@@ -1274,25 +1274,25 @@
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="J7" s="3">
         <v>39.115279999999998</v>
@@ -1301,13 +1301,13 @@
         <v>-77.564430000000002</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
@@ -1318,25 +1318,25 @@
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="J8" s="3">
         <v>40.741895</v>
@@ -1345,13 +1345,13 @@
         <v>-73.989307999999994</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
@@ -1362,38 +1362,38 @@
         <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K9" s="3"/>
       <c r="L9" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="62" x14ac:dyDescent="0.35">
@@ -1401,28 +1401,28 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J10" s="3">
         <v>39.108399900000002</v>
@@ -1431,13 +1431,13 @@
         <v>-77.565337</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="46.5" x14ac:dyDescent="0.35">
@@ -1445,28 +1445,28 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="J11" s="3">
         <v>39.114409999999999</v>
@@ -1475,13 +1475,13 @@
         <v>-77.540580000000006</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="62" x14ac:dyDescent="0.35">
@@ -1492,25 +1492,25 @@
         <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="J12" s="3">
         <v>39.115943000000001</v>
@@ -1519,13 +1519,13 @@
         <v>-77.581795999999997</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="31" x14ac:dyDescent="0.35">
@@ -1536,25 +1536,25 @@
         <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="J13" s="4">
         <v>39.114406199999998</v>
@@ -1563,13 +1563,13 @@
         <v>-77.567706299999998</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
@@ -1578,25 +1578,25 @@
         <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J14" s="3">
         <v>37.542472099999998</v>
@@ -1605,13 +1605,13 @@
         <v>-77.435912200000004</v>
       </c>
       <c r="L14" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="N14" s="6" t="s">
         <v>160</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="N14" s="6" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="31" x14ac:dyDescent="0.35">
@@ -1620,25 +1620,25 @@
         <v>5</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J15" s="3">
         <v>39.117853099999998</v>
@@ -1647,13 +1647,13 @@
         <v>-77.568151900000004</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
@@ -1662,25 +1662,25 @@
         <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J16" s="3">
         <v>37.610656959136698</v>
@@ -1689,13 +1689,13 @@
         <v>-77.340073015724201</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="31" x14ac:dyDescent="0.35">
@@ -1704,40 +1704,40 @@
         <v>5</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H17" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="N17" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
@@ -1745,41 +1745,41 @@
         <v>13</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="I18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="J18" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K18" s="4"/>
       <c r="L18" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="N18" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
@@ -1787,28 +1787,28 @@
         <v>14</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>32</v>
+        <v>172</v>
       </c>
       <c r="J19" s="3">
         <v>40.439779999999999</v>
@@ -1817,13 +1817,13 @@
         <v>-79.998869999999997</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N19" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="46.5" x14ac:dyDescent="0.35">
@@ -1831,43 +1831,43 @@
         <v>16</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="46.5" x14ac:dyDescent="0.35">
@@ -1875,43 +1875,43 @@
         <v>17</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I21" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="H21" s="3" t="s">
+      <c r="J21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N21" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N21" s="6" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="31" x14ac:dyDescent="0.35">
@@ -1919,43 +1919,43 @@
         <v>18</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="31" x14ac:dyDescent="0.35">
@@ -1963,43 +1963,43 @@
         <v>19</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="N23" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
@@ -2007,39 +2007,39 @@
         <v>20</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="N24" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
@@ -2047,28 +2047,28 @@
         <v>21</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J25" s="3">
         <v>40.407960000000003</v>
@@ -2077,13 +2077,13 @@
         <v>-79.909257999999994</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N25" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="31" x14ac:dyDescent="0.35">
@@ -2091,28 +2091,28 @@
         <v>22</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I26" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="J26" s="3">
         <v>40.405259100000002</v>
@@ -2121,13 +2121,13 @@
         <v>-79.829184400000003</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="N26" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="31" x14ac:dyDescent="0.35">
@@ -2135,28 +2135,28 @@
         <v>23</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D27" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I27" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="J27" s="3">
         <v>40.559510000000003</v>
@@ -2165,13 +2165,13 @@
         <v>-79.958669999999998</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N27" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
@@ -2179,19 +2179,19 @@
         <v>24</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
@@ -2207,19 +2207,19 @@
         <v>25</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>131</v>
-      </c>
       <c r="E29" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -2235,19 +2235,19 @@
         <v>26</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -2263,19 +2263,19 @@
         <v>27</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -2291,19 +2291,19 @@
         <v>28</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -2319,19 +2319,19 @@
         <v>29</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -2347,19 +2347,19 @@
         <v>30</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="E34" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
@@ -2375,19 +2375,19 @@
         <v>31</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -2403,19 +2403,19 @@
         <v>32</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C36" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="E36" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>

</xml_diff>

<commit_message>
Update erroneous entries in Juvenile Detention Excel File
</commit_message>
<xml_diff>
--- a/Qualitative_research/Research-Juvenile_Detention-New_col_added.xlsx
+++ b/Qualitative_research/Research-Juvenile_Detention-New_col_added.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyle9\Documents\New folder\2021_DSPG_Loudoun\Qualitative_research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\VT DSPG\R files\2021_DSPG_Loudoun\Qualitative_research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935DA122-EAC3-4AD4-B30E-D31D00C39B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FFC657-EDF2-4E1D-95B1-12AA57931FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{496A8450-741B-46B0-A040-55A896ED8080}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{496A8450-741B-46B0-A040-55A896ED8080}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="214">
   <si>
     <t>County</t>
   </si>
@@ -588,18 +588,9 @@
     <t>https://www.yearup.org/</t>
   </si>
   <si>
-    <t>Friends of Guest House</t>
-  </si>
-  <si>
-    <t>https://friendsofguesthouse.org/</t>
-  </si>
-  <si>
     <t>16-24</t>
   </si>
   <si>
-    <t>Provides shelter for homeless youth</t>
-  </si>
-  <si>
     <t>https://www.ccac.edu/academics/free-and-subsidized.php</t>
   </si>
   <si>
@@ -633,12 +624,6 @@
     <t>Erie, PA</t>
   </si>
   <si>
-    <t>incomes at or below 133% of the Federal Income Poverty Guidelines</t>
-  </si>
-  <si>
-    <t>https://www.dhs.pa.gov/healthchoices/Pages/HealthChoices.aspx</t>
-  </si>
-  <si>
     <t>The year up program is a year long professional development program focused on providing minorities between the ages of 18- 24 technical and other development skills and education.</t>
   </si>
   <si>
@@ -670,6 +655,55 @@
   </si>
   <si>
     <t>https://americorps.gov/serve/fit-finder/americorps-vista</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allegheny Couny residents who are or have applied to receive medicaid/third-party prescription coverage and make an adusted income of $500 dollars or less </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free psychiatric prescription medication </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allegheny County Office of Behavioral Health </t>
+  </si>
+  <si>
+    <t>https://www.alleghenycounty.us/WorkArea/linkit.aspx?LinkIdentifier=id&amp;ItemID=2147486416</t>
+  </si>
+  <si>
+    <t>A collection of programs available to Pennsylvania residents who recieve medicaid.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Programs designed to provide skills and knowledge needed to remain competitive in a variety of industries.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Awards commonwealth secondary school diplomas </t>
+  </si>
+  <si>
+    <t>Those who do not possess secondary diplomas after successful completion of 30-credit hours in relevant courses.</t>
+  </si>
+  <si>
+    <t>Community College of Allegheny County</t>
+  </si>
+  <si>
+    <t>Allegheny County youth with educational barriers</t>
+  </si>
+  <si>
+    <t>Individualized support for youth with educational barriers. The Liaison works within the framework of the Department of Human Services to coordinate continued education opportunities.</t>
+  </si>
+  <si>
+    <t>https://www.alleghenycounty.us/Human-Services/Resources/Education/DHS-Methods.aspx</t>
+  </si>
+  <si>
+    <t>https://www.ccac.edu/workforce/index.php</t>
+  </si>
+  <si>
+    <t>https://www.ccac.edu/admissions/ged.php</t>
+  </si>
+  <si>
+    <t>PortAuthority.org</t>
+  </si>
+  <si>
+    <t>Public transit agency in Alleghany Count</t>
   </si>
 </sst>
 </file>
@@ -728,10 +762,10 @@
       <name val="Roboto"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -757,9 +791,6 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -776,8 +807,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1095,1642 +1129,1690 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B741EA-BD98-4FD7-9B1C-17627FF53E8A}">
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="O38" sqref="O38"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="24.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="54.5703125" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1"/>
-    <col min="6" max="6" width="47.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
-    <col min="8" max="8" width="144.85546875" customWidth="1"/>
-    <col min="9" max="9" width="79.85546875" style="1" customWidth="1"/>
-    <col min="10" max="11" width="115.7109375" customWidth="1"/>
-    <col min="12" max="12" width="116.140625" customWidth="1"/>
-    <col min="13" max="13" width="99.85546875" customWidth="1"/>
-    <col min="14" max="14" width="75.7109375" customWidth="1"/>
-    <col min="15" max="15" width="46.85546875" customWidth="1"/>
-    <col min="16" max="16" width="111.42578125" customWidth="1"/>
+    <col min="1" max="2" width="24.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" customWidth="1"/>
+    <col min="4" max="4" width="54.54296875" customWidth="1"/>
+    <col min="5" max="5" width="23.1796875" customWidth="1"/>
+    <col min="6" max="6" width="47.453125" customWidth="1"/>
+    <col min="7" max="7" width="18.453125" customWidth="1"/>
+    <col min="8" max="8" width="144.81640625" customWidth="1"/>
+    <col min="9" max="9" width="91.81640625" style="3" customWidth="1"/>
+    <col min="10" max="11" width="115.7265625" customWidth="1"/>
+    <col min="12" max="12" width="116.1796875" customWidth="1"/>
+    <col min="13" max="13" width="99.81640625" customWidth="1"/>
+    <col min="14" max="14" width="75.7265625" customWidth="1"/>
+    <col min="15" max="15" width="46.81640625" customWidth="1"/>
+    <col min="16" max="16" width="111.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" cm="1">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" cm="1">
         <f t="array" ref="A2">_xlfn.SEQUENCE(,,1)</f>
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="2">
         <v>39.114409999999999</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="2">
         <v>-77.540580000000006</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="E3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="2">
         <v>39.114409999999999</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3" s="2">
         <v>-77.540581000000003</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="O3" s="10"/>
-    </row>
-    <row r="4" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="O3" s="9"/>
+    </row>
+    <row r="4" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="E4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="M4" s="3" t="s">
+      <c r="J4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="N4" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+    <row r="5" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="E5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <v>39.076819999999998</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="2">
         <v>-77.549896000000004</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="O5" s="3"/>
-    </row>
-    <row r="6" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="E6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="2">
         <v>39.114409999999999</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="2">
         <v>-77.540581000000003</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="N6" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+    <row r="7" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="E7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="2">
         <v>39.115279999999998</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="2">
         <v>-77.564430000000002</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="M7" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="N7" s="6" t="s">
+      <c r="N7" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="E8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="2">
         <v>40.741895</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="2">
         <v>-73.989307999999994</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="N8" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="E9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="M9" s="3" t="s">
+      <c r="J9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="M9" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="N9" s="6" t="s">
+      <c r="N9" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="63" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+    <row r="10" spans="1:15" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="E10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="2">
         <v>39.108399900000002</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="2">
         <v>-77.565337</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="M10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N10" s="6" t="s">
+      <c r="N10" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+    <row r="11" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="E11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="2">
         <v>39.114409999999999</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11" s="2">
         <v>-77.540580000000006</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="L11" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="M11" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="N11" s="6" t="s">
+      <c r="N11" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="O11" s="3"/>
-    </row>
-    <row r="12" spans="1:15" ht="63" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="O11" s="2"/>
+    </row>
+    <row r="12" spans="1:15" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="E12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="2">
         <v>39.115943000000001</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="2">
         <v>-77.581795999999997</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="L12" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="M12" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="N12" s="6" t="s">
+      <c r="N12" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="O12" s="3"/>
-    </row>
-    <row r="13" spans="1:15" ht="33" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="1:15" ht="32.5" x14ac:dyDescent="0.5">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="E13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="3">
         <v>39.114406199999998</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="3">
         <v>-77.567706299999998</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="L13" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="M13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="N13" s="6" t="s">
+      <c r="N13" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="O13" s="9"/>
-    </row>
-    <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3" t="s">
+      <c r="O13" s="8"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="3" t="s">
+      <c r="E14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="2">
         <v>37.542472099999998</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14" s="2">
         <v>-77.435912200000004</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="L14" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="M14" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="N14" s="6" t="s">
+      <c r="N14" s="5" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3" t="s">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" s="3" t="s">
+      <c r="E15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="2">
         <v>39.117853099999998</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K15" s="2">
         <v>-77.568151900000004</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="L15" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="M15" s="3" t="s">
+      <c r="M15" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="N15" s="5" t="s">
+      <c r="N15" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="O15" s="3"/>
-    </row>
-    <row r="16" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3" t="s">
+      <c r="O15" s="2"/>
+    </row>
+    <row r="16" spans="1:15" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="3" t="s">
+      <c r="E16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="2">
         <v>37.610656959136698</v>
       </c>
-      <c r="K16" s="3">
+      <c r="K16" s="2">
         <v>-77.340073015724201</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="L16" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="M16" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="N16" s="8" t="s">
+      <c r="N16" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="O16" s="3"/>
-    </row>
-    <row r="17" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3" t="s">
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" s="3" t="s">
+      <c r="E17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="J17" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="L17" s="3" t="s">
+      <c r="J17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="M17" s="3" t="s">
+      <c r="M17" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="N17" s="3" t="s">
+      <c r="N17" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
         <v>13</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="4" t="s">
+      <c r="E18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J18" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="M18" s="4" t="s">
+      <c r="J18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="M18" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="N18" s="6" t="s">
+      <c r="N18" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="O18" s="4"/>
-    </row>
-    <row r="19" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
         <v>14</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" s="3" t="s">
+      <c r="E19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="2">
         <v>40.439779999999999</v>
       </c>
-      <c r="K19" s="3">
+      <c r="K19" s="2">
         <v>-79.998869999999997</v>
       </c>
-      <c r="L19" s="7" t="s">
+      <c r="L19" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="M19" s="3" t="s">
+      <c r="M19" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="N19" s="5" t="s">
+      <c r="N19" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="O19" s="3"/>
-    </row>
-    <row r="20" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="O19" s="2"/>
+    </row>
+    <row r="20" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
         <v>16</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F20" s="3" t="s">
+      <c r="E20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="I20" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="M20" s="3" t="s">
+      <c r="J20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="M20" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N20" s="5" t="s">
+      <c r="N20" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="O20" s="3"/>
-    </row>
-    <row r="21" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="O20" s="2"/>
+    </row>
+    <row r="21" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
         <v>17</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F21" s="3" t="s">
+      <c r="E21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="I21" s="4" t="s">
+      <c r="I21" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J21" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="M21" s="3" t="s">
+      <c r="J21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="M21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N21" s="6" t="s">
+      <c r="N21" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="O21" s="3"/>
-    </row>
-    <row r="22" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="O21" s="2"/>
+    </row>
+    <row r="22" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
         <v>18</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="3" t="s">
+      <c r="E22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="I22" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J22" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="L22" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="M22" s="3" t="s">
+      <c r="J22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="M22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N22" s="6" t="s">
+      <c r="N22" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="O22" s="3"/>
-    </row>
-    <row r="23" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+      <c r="O22" s="2"/>
+    </row>
+    <row r="23" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
         <v>19</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="3" t="s">
+      <c r="E23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="I23" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J23" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="L23" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="M23" s="3" t="s">
+      <c r="J23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="M23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N23" s="5" t="s">
+      <c r="N23" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="O23" s="3"/>
-    </row>
-    <row r="24" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+      <c r="O23" s="2"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A24" s="2">
         <v>20</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F24" s="3" t="s">
+      <c r="E24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H24" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="I24" s="4" t="s">
+      <c r="I24" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3" t="s">
+      <c r="J24" s="2"/>
+      <c r="K24" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N24" s="6" t="s">
+      <c r="N24" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
         <v>21</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25" s="3" t="s">
+      <c r="E25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="H25" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="I25" s="4" t="s">
+      <c r="I25" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="2">
         <v>40.407960000000003</v>
       </c>
-      <c r="K25" s="3">
+      <c r="K25" s="2">
         <v>-79.909257999999994</v>
       </c>
-      <c r="L25" s="4" t="s">
+      <c r="L25" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="M25" s="3" t="s">
+      <c r="M25" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="N25" s="5" t="s">
+      <c r="N25" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="O25" s="3"/>
-    </row>
-    <row r="26" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+      <c r="O25" s="2"/>
+    </row>
+    <row r="26" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+      <c r="A26" s="2">
         <v>22</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F26" s="3" t="s">
+      <c r="E26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="H26" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="I26" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="2">
         <v>40.405259100000002</v>
       </c>
-      <c r="K26" s="3">
+      <c r="K26" s="2">
         <v>-79.829184400000003</v>
       </c>
-      <c r="L26" s="4" t="s">
+      <c r="L26" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="M26" s="3" t="s">
+      <c r="M26" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="N26" s="6" t="s">
+      <c r="N26" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="O26" s="3"/>
-    </row>
-    <row r="27" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+      <c r="O26" s="2"/>
+    </row>
+    <row r="27" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+      <c r="A27" s="2">
         <v>23</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F27" s="3" t="s">
+      <c r="E27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G27" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="I27" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27" s="2">
         <v>40.559510000000003</v>
       </c>
-      <c r="K27" s="3">
+      <c r="K27" s="2">
         <v>-79.958669999999998</v>
       </c>
-      <c r="L27" s="4" t="s">
+      <c r="L27" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="M27" s="3" t="s">
+      <c r="M27" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="N27" s="6" t="s">
+      <c r="N27" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="O27" s="3"/>
-    </row>
-    <row r="28" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
+      <c r="O27" s="2"/>
+    </row>
+    <row r="28" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+      <c r="A28" s="2">
         <v>24</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F28" s="3" t="s">
+      <c r="E28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="O28" s="2"/>
+      <c r="Q28" s="2"/>
+    </row>
+    <row r="29" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="2">
+        <v>25</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G29" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="J29" s="2">
+        <v>40.427699871314402</v>
+      </c>
+      <c r="K29" s="2">
+        <v>-80.135979742535696</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="P29" s="2"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A30" s="2">
+        <v>26</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="J30" s="2">
+        <v>40.427699871314402</v>
+      </c>
+      <c r="K30" s="2">
+        <v>-80.135979742535696</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+      <c r="A31" s="2">
+        <v>27</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="J31" s="2">
+        <v>40.427699871314402</v>
+      </c>
+      <c r="K31" s="2">
+        <v>-80.135979742535696</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="M31" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A32" s="2">
+        <v>28</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="J32" s="2">
+        <v>40.427699871314402</v>
+      </c>
+      <c r="K32" s="2">
+        <v>-80.135979742535696</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="M32" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A33" s="2">
+        <v>29</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="M33" s="2"/>
+      <c r="N33" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A34" s="2">
+        <v>30</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="M34" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="H28" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3" t="s">
+      <c r="N34" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A35" s="2">
+        <v>31</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H35" s="2"/>
+      <c r="I35" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A36" s="2">
+        <v>32</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="31" x14ac:dyDescent="0.35">
+      <c r="A37" s="2">
+        <v>33</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="N28" s="3" t="s">
+      <c r="E37" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="N37" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="O28" s="3"/>
-      <c r="Q28" s="3"/>
-    </row>
-    <row r="29" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>25</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F29" s="3" t="s">
+    </row>
+    <row r="38" spans="1:14" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="2">
+        <v>34</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="I29" s="4"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="N29" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="P29" s="3"/>
-    </row>
-    <row r="30" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>26</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-    </row>
-    <row r="31" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <v>27</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G31" s="3" t="s">
+      <c r="G38" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H31" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="J31" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="K31" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="L31" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="M31" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="N31" s="3" t="s">
+      <c r="H38" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="J38" s="2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
-        <v>28</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="J32" s="3">
-        <v>40.427699871314402</v>
-      </c>
-      <c r="K32" s="3">
-        <v>-80.135979742535696</v>
-      </c>
-      <c r="L32" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="M32" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="N32" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
-        <v>29</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-    </row>
-    <row r="34" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
-        <v>30</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="I34" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="K34" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="L34" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="M34" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="N34" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
-        <v>31</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="H35" s="3" t="s">
+      <c r="K38" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="M38" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="I35" s="4"/>
-      <c r="J35" s="3">
-        <v>42.126175156561303</v>
-      </c>
-      <c r="K35" s="3">
-        <v>-80.086767930687998</v>
-      </c>
-      <c r="L35" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
-    </row>
-    <row r="36" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
-        <v>32</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G36" s="3">
-        <v>1</v>
-      </c>
-      <c r="H36" s="3"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
-        <v>33</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="H37" s="3" t="s">
+      <c r="N38" s="11" t="s">
         <v>197</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="J37" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="K37" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="L37" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="M37" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="N37" s="13" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
-        <v>34</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="K38" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="L38" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="M38" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="N38" s="13" t="s">
-        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2765,8 +2847,10 @@
     <hyperlink ref="N36" r:id="rId27" xr:uid="{14713502-818E-483A-89A8-06F5F62DD4D1}"/>
     <hyperlink ref="N37" r:id="rId28" xr:uid="{A7CE5E6C-4702-4C69-9D91-DBE4E273431B}"/>
     <hyperlink ref="N38" r:id="rId29" xr:uid="{82510A41-0E4E-470F-B876-BB87D0B5D25A}"/>
+    <hyperlink ref="N28" r:id="rId30" xr:uid="{189F304E-5F5E-412D-9BB0-1F06E2D2997E}"/>
+    <hyperlink ref="N33" r:id="rId31" display="https://www.portauthority.org/" xr:uid="{C880A428-41C0-47D5-8FDC-9FC7139585CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId30"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added improved descriptions to map
</commit_message>
<xml_diff>
--- a/Qualitative_research/Research-Juvenile_Detention-New_col_added.xlsx
+++ b/Qualitative_research/Research-Juvenile_Detention-New_col_added.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\VT DSPG\R files\2021_DSPG_Loudoun\Qualitative_research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC7C693-5BB3-42E9-A3FC-B042EB8AFFA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BA4496-623D-425F-A2C4-E5D18D02EE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{496A8450-741B-46B0-A040-55A896ED8080}"/>
   </bookViews>
@@ -1107,8 +1107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B741EA-BD98-4FD7-9B1C-17627FF53E8A}">
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="O3" s="9"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2272,7 +2272,7 @@
       </c>
       <c r="O26" s="2"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>23</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>27</v>
       </c>

</xml_diff>